<commit_message>
proper scoring sheet PDF
</commit_message>
<xml_diff>
--- a/teammatch2x8.xlsx
+++ b/teammatch2x8.xlsx
@@ -473,22 +473,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PH64</t>
+          <t>PH16</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PH44</t>
+          <t>PH87</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PH98</t>
+          <t>PH31</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PH44</t>
+          <t>PH89</t>
         </is>
       </c>
     </row>
@@ -500,22 +500,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PH34</t>
+          <t>PH19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PH88</t>
+          <t>PH82</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PH95</t>
+          <t>PH79</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>PH64</t>
+          <t>PH89</t>
         </is>
       </c>
     </row>

</xml_diff>